<commit_message>
Atualização dos dados e melhorias no codigo
</commit_message>
<xml_diff>
--- a/Dados/01_abr.xlsx
+++ b/Dados/01_abr.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -345,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -354,31 +367,43 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>americana</t>
-        </is>
-      </c>
-      <c r="B1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C1" t="inlineStr"/>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 2</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>aracatuba</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>2</v>
-      </c>
-      <c r="C2" t="inlineStr"/>
+          <t>municipio</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>CASOS</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ÓBITOS</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>aruja</t>
+          <t>americana</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -389,18 +414,18 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>barueri</t>
+          <t>aracatuba</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>bauru</t>
+          <t>aruja</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -411,42 +436,40 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>brodowski</t>
+          <t>barueri</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>cachoeira paulista</t>
+          <t>bauru</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>caieiras</t>
+          <t>brodowski</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>11</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>cajamar</t>
+          <t>cachoeira paulista</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -457,11 +480,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>campinas</t>
+          <t>caieiras</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
@@ -470,101 +493,101 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>carapicuiba</t>
+          <t>cajamar</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>cotia</t>
+          <t>campinas</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>diadema</t>
+          <t>carapicuiba</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>embu das artes</t>
+          <t>cotia</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ferraz de vasconcelos</t>
+          <t>diadema</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>franco da rocha</t>
+          <t>embu das artes</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>guaruja</t>
+          <t>ferraz de vasconcelos</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>guarulhos</t>
+          <t>franco da rocha</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>25</v>
-      </c>
-      <c r="C18" t="n">
-        <v>2</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>hortolandia</t>
+          <t>guaruja</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -575,18 +598,20 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>indaiatuba</t>
+          <t>guarulhos</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>2</v>
-      </c>
-      <c r="C20" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="C20" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>iracemapolis</t>
+          <t>hortolandia</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -597,7 +622,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>itanhaem</t>
+          <t>indaiatuba</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -608,106 +633,106 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>itapecerica da serra</t>
+          <t>iracemapolis</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>itapevi</t>
+          <t>itanhaem</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>itaquaquecetuba</t>
+          <t>itapecerica da serra</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>itupeva</t>
+          <t>itapevi</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>jaguariuna</t>
+          <t>itaquaquecetuba</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>jandira</t>
+          <t>itupeva</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>jundiai</t>
+          <t>jaguariuna</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>lencois paulista</t>
+          <t>jandira</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>limeira</t>
+          <t>jundiai</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>louveira</t>
+          <t>lencois paulista</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -718,7 +743,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>mairipora</t>
+          <t>limeira</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -729,7 +754,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>matao</t>
+          <t>louveira</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -740,64 +765,62 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>maua</t>
+          <t>mairipora</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>mogi das cruzes</t>
+          <t>matao</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>mogi guacu</t>
+          <t>maua</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>nova odessa</t>
+          <t>mogi das cruzes</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>osasco</t>
+          <t>mogi guacu</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>43</v>
-      </c>
-      <c r="C39" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>paulinia</t>
+          <t>nova odessa</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -808,29 +831,31 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>penapolis</t>
+          <t>osasco</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>1</v>
-      </c>
-      <c r="C41" t="inlineStr"/>
+        <v>43</v>
+      </c>
+      <c r="C41" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>piracicaba</t>
+          <t>paulinia</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>pirajui</t>
+          <t>penapolis</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -841,18 +866,18 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>poa</t>
+          <t>piracicaba</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>porto feliz</t>
+          <t>pirajui</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -863,7 +888,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>praia grande</t>
+          <t>poa</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -874,7 +899,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>ribeirao pires</t>
+          <t>porto feliz</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -885,20 +910,18 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>ribeirao preto</t>
+          <t>praia grande</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>8</v>
-      </c>
-      <c r="C48" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>rio claro</t>
+          <t>ribeirao pires</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -909,18 +932,20 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>salto de pirapora</t>
+          <t>ribeirao preto</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>1</v>
-      </c>
-      <c r="C50" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>santa isabel</t>
+          <t>rio claro</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -931,46 +956,44 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>santana de parnaiba</t>
+          <t>salto de pirapora</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="C52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>santo andre</t>
+          <t>santa isabel</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>51</v>
-      </c>
-      <c r="C53" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>santos</t>
+          <t>santana de parnaiba</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>sao bernardo do campo</t>
+          <t>santo andre</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" t="n">
         <v>2</v>
@@ -979,101 +1002,101 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>sao caetano do sul</t>
+          <t>santos</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>32</v>
-      </c>
-      <c r="C56" t="n">
-        <v>1</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>sao jose do rio pardo</t>
+          <t>sao bernardo do campo</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>1</v>
-      </c>
-      <c r="C57" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>sao jose do rio preto</t>
+          <t>sao caetano do sul</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>7</v>
-      </c>
-      <c r="C58" t="inlineStr"/>
+        <v>32</v>
+      </c>
+      <c r="C58" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>sao jose dos campos</t>
+          <t>sao jose do rio pardo</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="C59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>sao paulo</t>
+          <t>sao jose do rio preto</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>2418</v>
-      </c>
-      <c r="C60" t="n">
-        <v>144</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>sao pedro</t>
+          <t>sao jose dos campos</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>sao sebastiao</t>
+          <t>sao paulo</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>3</v>
+        <v>2418</v>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>sao vicente</t>
+          <t>sao pedro</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>sorocaba</t>
+          <t>sao sebastiao</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1086,24 +1109,22 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>suzano</t>
+          <t>sao vicente</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>4</v>
-      </c>
-      <c r="C65" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>taboao da serra</t>
+          <t>sorocaba</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C66" t="n">
         <v>1</v>
@@ -1112,29 +1133,33 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>tatui</t>
+          <t>suzano</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
-      </c>
-      <c r="C67" t="inlineStr"/>
+        <v>4</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>taubate</t>
+          <t>taboao da serra</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>1</v>
-      </c>
-      <c r="C68" t="inlineStr"/>
+        <v>22</v>
+      </c>
+      <c r="C68" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>valinhos</t>
+          <t>tatui</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1145,20 +1170,18 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>vargem grande paulista</t>
+          <t>taubate</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>2</v>
-      </c>
-      <c r="C70" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>vinhedo</t>
+          <t>valinhos</t>
         </is>
       </c>
       <c r="B71" t="n">
@@ -1169,24 +1192,70 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>votorantim</t>
+          <t>vargem grande paulista</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>1</v>
-      </c>
-      <c r="C72" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="C72" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>vinhedo</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>1</v>
+      </c>
+      <c r="C73" t="inlineStr"/>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>votorantim</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>1</v>
+      </c>
+      <c r="C74" t="inlineStr"/>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
           <t>votuporanga</t>
         </is>
       </c>
-      <c r="B73" t="n">
-        <v>1</v>
-      </c>
-      <c r="C73" t="inlineStr"/>
+      <c r="B75" t="n">
+        <v>1</v>
+      </c>
+      <c r="C75" t="inlineStr"/>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>outros paises</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>33</v>
+      </c>
+      <c r="C76" t="inlineStr"/>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>outros estados</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>22</v>
+      </c>
+      <c r="C77" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Atualização dos dados, criação dos procedimentos de limpeza como funções e unificação da análise
Os arquivos com as funções utilizadas na limpeza e criação dos dataframes foram convertidos em funções simples e importadas dentro do arquivo de análise onde são utilizadas e depois procedemos à análise
</commit_message>
<xml_diff>
--- a/Dados/01_abr.xlsx
+++ b/Dados/01_abr.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -386,24 +386,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>municipio</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>CASOS</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ÓBITOS</t>
-        </is>
-      </c>
+          <t>americana</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>americana</t>
+          <t>aracatuba</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -414,7 +408,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>aracatuba</t>
+          <t>aruja</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -425,40 +419,40 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>aruja</t>
+          <t>barueri</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>barueri</t>
+          <t>bauru</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="C6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>bauru</t>
+          <t>brodowski</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>brodowski</t>
+          <t>cachoeira paulista</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -469,226 +463,226 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>cachoeira paulista</t>
+          <t>caieiras</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>caieiras</t>
+          <t>cajamar</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>11</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>cajamar</t>
+          <t>campinas</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
+        <v>22</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>campinas</t>
+          <t>carapicuiba</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>22</v>
-      </c>
-      <c r="C12" t="n">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>carapicuiba</t>
+          <t>cotia</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
+        <v>21</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>cotia</t>
+          <t>diadema</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>21</v>
-      </c>
-      <c r="C14" t="n">
-        <v>2</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>diadema</t>
+          <t>embu das artes</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>8</v>
       </c>
-      <c r="C15" t="inlineStr"/>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>embu das artes</t>
+          <t>ferraz de vasconcelos</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>8</v>
-      </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ferraz de vasconcelos</t>
+          <t>franco da rocha</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>franco da rocha</t>
+          <t>guaruja</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>guaruja</t>
+          <t>guarulhos</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr"/>
+        <v>25</v>
+      </c>
+      <c r="C19" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>guarulhos</t>
+          <t>hortolandia</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>25</v>
-      </c>
-      <c r="C20" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>hortolandia</t>
+          <t>indaiatuba</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>indaiatuba</t>
+          <t>iracemapolis</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>iracemapolis</t>
+          <t>itanhaem</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>itanhaem</t>
+          <t>itapecerica da serra</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>itapecerica da serra</t>
+          <t>itapevi</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>itapevi</t>
+          <t>itaquaquecetuba</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>itaquaquecetuba</t>
+          <t>itupeva</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>itupeva</t>
+          <t>jaguariuna</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -699,117 +693,117 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>jaguariuna</t>
+          <t>jandira</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>jandira</t>
+          <t>jundiai</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>jundiai</t>
+          <t>lencois paulista</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>lencois paulista</t>
+          <t>limeira</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>limeira</t>
+          <t>louveira</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>louveira</t>
+          <t>mairipora</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>mairipora</t>
+          <t>matao</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>matao</t>
+          <t>maua</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>maua</t>
+          <t>mogi das cruzes</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>mogi das cruzes</t>
+          <t>mogi guacu</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>mogi guacu</t>
+          <t>nova odessa</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -820,31 +814,31 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>nova odessa</t>
+          <t>osasco</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>1</v>
-      </c>
-      <c r="C40" t="inlineStr"/>
+        <v>43</v>
+      </c>
+      <c r="C40" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>osasco</t>
+          <t>paulinia</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>43</v>
-      </c>
-      <c r="C41" t="n">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>paulinia</t>
+          <t>penapolis</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -855,29 +849,29 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>penapolis</t>
+          <t>piracicaba</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>piracicaba</t>
+          <t>pirajui</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>pirajui</t>
+          <t>poa</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -888,7 +882,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>poa</t>
+          <t>porto feliz</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -899,7 +893,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>porto feliz</t>
+          <t>praia grande</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -910,7 +904,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>praia grande</t>
+          <t>ribeirao pires</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -921,31 +915,31 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>ribeirao pires</t>
+          <t>ribeirao preto</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>1</v>
-      </c>
-      <c r="C49" t="inlineStr"/>
+        <v>8</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>ribeirao preto</t>
+          <t>rio claro</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>8</v>
-      </c>
-      <c r="C50" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>rio claro</t>
+          <t>salto de pirapora</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -956,7 +950,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>salto de pirapora</t>
+          <t>santa isabel</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -967,164 +961,166 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>santa isabel</t>
+          <t>santana de parnaiba</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="C53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>santana de parnaiba</t>
+          <t>santo andre</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>18</v>
-      </c>
-      <c r="C54" t="inlineStr"/>
+        <v>51</v>
+      </c>
+      <c r="C54" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>santo andre</t>
+          <t>santos</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>51</v>
-      </c>
-      <c r="C55" t="n">
-        <v>2</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="C55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>santos</t>
+          <t>sao bernardo do campo</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>23</v>
-      </c>
-      <c r="C56" t="inlineStr"/>
+        <v>52</v>
+      </c>
+      <c r="C56" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>sao bernardo do campo</t>
+          <t>sao caetano do sul</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C57" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>sao caetano do sul</t>
+          <t>sao jose do rio pardo</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>32</v>
-      </c>
-      <c r="C58" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>sao jose do rio pardo</t>
+          <t>sao jose do rio preto</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>sao jose do rio preto</t>
+          <t>sao jose dos campos</t>
         </is>
       </c>
       <c r="B60" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>sao jose dos campos</t>
+          <t>sao paulo</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>12</v>
-      </c>
-      <c r="C61" t="inlineStr"/>
+        <v>2418</v>
+      </c>
+      <c r="C61" t="n">
+        <v>144</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>sao paulo</t>
+          <t>sao pedro</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2418</v>
-      </c>
-      <c r="C62" t="n">
-        <v>144</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>sao pedro</t>
+          <t>sao sebastiao</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>1</v>
-      </c>
-      <c r="C63" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="C63" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>sao sebastiao</t>
+          <t>sao vicente</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>3</v>
-      </c>
-      <c r="C64" t="n">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>sao vicente</t>
+          <t>sorocaba</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>2</v>
-      </c>
-      <c r="C65" t="inlineStr"/>
+        <v>3</v>
+      </c>
+      <c r="C65" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>sorocaba</t>
+          <t>suzano</t>
         </is>
       </c>
       <c r="B66" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C66" t="n">
         <v>1</v>
@@ -1133,11 +1129,11 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>suzano</t>
+          <t>taboao da serra</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C67" t="n">
         <v>1</v>
@@ -1146,20 +1142,18 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>taboao da serra</t>
+          <t>tatui</t>
         </is>
       </c>
       <c r="B68" t="n">
-        <v>22</v>
-      </c>
-      <c r="C68" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>tatui</t>
+          <t>taubate</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1170,7 +1164,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>taubate</t>
+          <t>valinhos</t>
         </is>
       </c>
       <c r="B70" t="n">
@@ -1181,31 +1175,31 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>valinhos</t>
+          <t>vargem grande paulista</t>
         </is>
       </c>
       <c r="B71" t="n">
-        <v>1</v>
-      </c>
-      <c r="C71" t="inlineStr"/>
+        <v>2</v>
+      </c>
+      <c r="C71" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>vargem grande paulista</t>
+          <t>vinhedo</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>2</v>
-      </c>
-      <c r="C72" t="n">
-        <v>1</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="C72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>vinhedo</t>
+          <t>votorantim</t>
         </is>
       </c>
       <c r="B73" t="n">
@@ -1216,46 +1210,13 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>votorantim</t>
+          <t>votuporanga</t>
         </is>
       </c>
       <c r="B74" t="n">
         <v>1</v>
       </c>
       <c r="C74" t="inlineStr"/>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>votuporanga</t>
-        </is>
-      </c>
-      <c r="B75" t="n">
-        <v>1</v>
-      </c>
-      <c r="C75" t="inlineStr"/>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>outros paises</t>
-        </is>
-      </c>
-      <c r="B76" t="n">
-        <v>33</v>
-      </c>
-      <c r="C76" t="inlineStr"/>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>outros estados</t>
-        </is>
-      </c>
-      <c r="B77" t="n">
-        <v>22</v>
-      </c>
-      <c r="C77" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>